<commit_message>
Tidying up the folder
</commit_message>
<xml_diff>
--- a/SQL/Analysis/Cluster_Count/Compliant_Clusters_Counts_with_names.xlsx
+++ b/SQL/Analysis/Cluster_Count/Compliant_Clusters_Counts_with_names.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD2712E-4358-46EA-A33E-CC71B58B6D29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCAFB17-7537-408D-8173-76F0F3C1B0CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="165" windowWidth="14070" windowHeight="5070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$C$1</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>final_cluster</t>
   </si>
@@ -95,14 +96,28 @@
   </si>
   <si>
     <t>3-way match, invoice before GR (without SRM, Item Type: Subcontracting)</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Precision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -126,13 +141,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="A1:C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -566,4 +607,190 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6411F5F-79EA-422E-9D7A-71DEC7C9740E}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="70.89453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>77.3</v>
+      </c>
+      <c r="D2">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>95.8</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>88.6</v>
+      </c>
+      <c r="D4">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>95</v>
+      </c>
+      <c r="D5">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>95.4</v>
+      </c>
+      <c r="D6">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>91.3</v>
+      </c>
+      <c r="D7">
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>97.9</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>90.3</v>
+      </c>
+      <c r="D9">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>91.6</v>
+      </c>
+      <c r="D10">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>97</v>
+      </c>
+      <c r="D11">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>